<commit_message>
manual prototype with made-up excels
</commit_message>
<xml_diff>
--- a/data_migration_try/empty.xlsx
+++ b/data_migration_try/empty.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efrag-my.sharepoint.com/personal/andrea_baschiera_efrag_org/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efrag-my.sharepoint.com/personal/andrea_baschiera_efrag_org/Documents/Desktop/PaperTeam/data_migration_try/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93D8E532-4386-4181-B139-6AB1D43CCADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{93D8E532-4386-4181-B139-6AB1D43CCADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8822D3B6-41B2-4E98-8251-472EB2D89704}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D75E74CA-AD54-4075-AFC2-364A1D05B28E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D75E74CA-AD54-4075-AFC2-364A1D05B28E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="number">Sheet1!$C$7</definedName>
+    <definedName name="stringa">Sheet1!$H$8:$H$11</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -413,7 +417,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>